<commit_message>
Fixed a few things There were a few things in the editing that need to happen Hopefully this will help
</commit_message>
<xml_diff>
--- a/Data/Power House Data.xlsx
+++ b/Data/Power House Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Barhoum Karam\Documents\For Github\LebanonElectricity\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B707F9-E788-4F21-A6CC-9234F412076F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39403EEF-04F4-46D9-9100-8818414619FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F6530CF5-1846-4A26-8384-049B0E703116}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="Villages of Lebanon" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$B$79</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Villages of Lebanon'!$A$1:$D$1629</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">PowerHousesData!$A$1:$D$994</definedName>
   </definedNames>
@@ -39324,9 +39325,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B9CCD25-7D1F-4028-A1F6-20EBBCA6E588}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A79" sqref="A2:A79"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -39358,7 +39362,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>912</v>
       </c>
@@ -39366,7 +39370,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>594</v>
       </c>
@@ -39414,7 +39418,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -39438,7 +39442,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -39446,7 +39450,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>851</v>
       </c>
@@ -39486,7 +39490,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>996</v>
       </c>
@@ -39510,7 +39514,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>892</v>
       </c>
@@ -39518,7 +39522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>210</v>
       </c>
@@ -39574,7 +39578,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>179</v>
       </c>
@@ -39598,7 +39602,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>678</v>
       </c>
@@ -39606,7 +39610,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>495</v>
       </c>
@@ -39630,7 +39634,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>812</v>
       </c>
@@ -39638,7 +39642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>103</v>
       </c>
@@ -39758,7 +39762,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>427</v>
       </c>
@@ -39806,7 +39810,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>394</v>
       </c>
@@ -39838,7 +39842,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>598</v>
       </c>
@@ -39854,7 +39858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>535</v>
       </c>
@@ -39918,7 +39922,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>704</v>
       </c>
@@ -39926,7 +39930,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>713</v>
       </c>
@@ -39942,7 +39946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>717</v>
       </c>
@@ -39950,7 +39954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>810</v>
       </c>
@@ -39971,6 +39975,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B79" xr:uid="{3B9CCD25-7D1F-4028-A1F6-20EBBCA6E588}">
+    <filterColumn colId="1">
+      <customFilters and="1">
+        <customFilter operator="greaterThanOrEqual" val="4"/>
+        <customFilter operator="lessThanOrEqual" val="22"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>